<commit_message>
update positional_accuracy and other details in readme
</commit_message>
<xml_diff>
--- a/data-raw/IGC_sample.xlsx
+++ b/data-raw/IGC_sample.xlsx
@@ -396,7 +396,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1020</v>
+        <v>1063</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -404,20 +404,20 @@
         </is>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>liga</t>
+          <t>bella</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ligas</t>
+          <t>bella</t>
         </is>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -425,7 +425,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>1107</v>
+        <v>545</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -433,16 +433,16 @@
         </is>
       </c>
       <c r="C3">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>facha</t>
+          <t>veraz</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>facha</t>
+          <t>veraz</t>
         </is>
       </c>
       <c r="F3">
@@ -454,7 +454,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>525</v>
+        <v>1107</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>94</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>laúd</t>
+          <t>facha</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>laúd</t>
+          <t>facha</t>
         </is>
       </c>
       <c r="F4">
@@ -483,7 +483,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>540</v>
+        <v>573</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -491,16 +491,16 @@
         </is>
       </c>
       <c r="C5">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>capa</t>
+          <t>leña</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>capa</t>
+          <t>leña</t>
         </is>
       </c>
       <c r="F5">
@@ -512,7 +512,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>1015</v>
+        <v>627</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -520,16 +520,16 @@
         </is>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>bario</t>
+          <t>raya</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>barios</t>
+          <t>ya, ca, raya</t>
         </is>
       </c>
       <c r="F6">
@@ -541,7 +541,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>1063</v>
+        <v>558</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>bella</t>
+          <t>patria</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>bella</t>
+          <t>patria</t>
         </is>
       </c>
       <c r="F7">
@@ -570,7 +570,7 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>612</v>
+        <v>527</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -578,16 +578,16 @@
         </is>
       </c>
       <c r="C8">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>rape</t>
+          <t>labor</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>rape</t>
+          <t>labor</t>
         </is>
       </c>
       <c r="F8">
@@ -599,7 +599,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>598</v>
+        <v>522</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -607,20 +607,20 @@
         </is>
       </c>
       <c r="C9">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>cobra</t>
+          <t>veloz</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>cobra</t>
+          <t>ver, lo, feloz, lelo, veloz</t>
         </is>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>569</v>
+        <v>1084</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -636,20 +636,20 @@
         </is>
       </c>
       <c r="C10">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>tonel</t>
+          <t>pina</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>tonel</t>
+          <t>pilas, pilas, pinas</t>
         </is>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>738</v>
+        <v>668</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -665,16 +665,16 @@
         </is>
       </c>
       <c r="C11">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>perfume</t>
+          <t>vigente</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>perfume</t>
+          <t>vigente</t>
         </is>
       </c>
       <c r="F11">
@@ -686,7 +686,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>1216</v>
+        <v>672</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -694,16 +694,16 @@
         </is>
       </c>
       <c r="C12">
-        <v>83</v>
+        <v>36</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>mollera</t>
+          <t>caída</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>mollera</t>
+          <t>caída</t>
         </is>
       </c>
       <c r="F12">
@@ -715,7 +715,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>637</v>
+        <v>1226</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -723,20 +723,20 @@
         </is>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>rellano</t>
+          <t>carajo</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>rellano</t>
+          <t>garajo, carajo</t>
         </is>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>1202</v>
+        <v>647</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -752,16 +752,16 @@
         </is>
       </c>
       <c r="C14">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>divorcio</t>
+          <t>aspecto</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>divorcio</t>
+          <t>aspecto</t>
         </is>
       </c>
       <c r="F14">
@@ -773,7 +773,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>747</v>
+        <v>690</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -781,28 +781,28 @@
         </is>
       </c>
       <c r="C15">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>congreso</t>
+          <t>rechazo</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>combreso</t>
+          <t>rechazo</t>
         </is>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>1185</v>
+        <v>728</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -810,20 +810,20 @@
         </is>
       </c>
       <c r="C16">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>retraso</t>
+          <t>concorde</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>retaso, retraso</t>
+          <t>concorde</t>
         </is>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -831,7 +831,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>1146</v>
+        <v>1253</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -839,16 +839,16 @@
         </is>
       </c>
       <c r="C17">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ligero</t>
+          <t>judía</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>ligero</t>
+          <t>judía</t>
         </is>
       </c>
       <c r="F17">
@@ -860,7 +860,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>717</v>
+        <v>710</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -868,16 +868,16 @@
         </is>
       </c>
       <c r="C18">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>regreso</t>
+          <t>almuerzo</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>regreso</t>
+          <t>almuerzo</t>
         </is>
       </c>
       <c r="F18">
@@ -889,7 +889,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>684</v>
+        <v>756</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -897,16 +897,16 @@
         </is>
       </c>
       <c r="C19">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>cabello</t>
+          <t>judía</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>cabello</t>
+          <t>judía</t>
         </is>
       </c>
       <c r="F19">
@@ -918,7 +918,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>955</v>
+        <v>940</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -926,16 +926,16 @@
         </is>
       </c>
       <c r="C20">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>supermercado</t>
+          <t>distinto</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>supermercado</t>
+          <t>distinto</t>
         </is>
       </c>
       <c r="F20">
@@ -947,7 +947,7 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>1260</v>
+        <v>1332</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -955,20 +955,20 @@
         </is>
       </c>
       <c r="C21">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>telefónica</t>
+          <t>preparatoria</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>telefónica</t>
+          <t>pre, pe, prepar, preparotoria, preparatoria</t>
         </is>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>875</v>
+        <v>840</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -984,28 +984,28 @@
         </is>
       </c>
       <c r="C22">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>preparatoria</t>
+          <t>inundación</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>pere, p, pe, prepara, preparatoria, preparatoria</t>
+          <t>unun, unincia, unin, unenzación, undiz, undi, uni, unde, indi, ninunación, indunación, indunaz, indininun, indi, indu, indunización</t>
         </is>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1296</v>
+        <v>1390</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1013,28 +1013,28 @@
         </is>
       </c>
       <c r="C23">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>mula</t>
+          <t>carnicería</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>mula</t>
+          <t>carnifería</t>
         </is>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>1370</v>
+        <v>1420</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1042,20 +1042,20 @@
         </is>
       </c>
       <c r="C24">
-        <v>117</v>
+        <v>167</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>portaaviones</t>
+          <t>volcán</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>pro, porva, portaaviones</t>
+          <t>volcán</t>
         </is>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>1269</v>
+        <v>1289</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1071,16 +1071,16 @@
         </is>
       </c>
       <c r="C25">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>cálida</t>
+          <t>economía</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>cálida</t>
+          <t>economía</t>
         </is>
       </c>
       <c r="F25">
@@ -1092,7 +1092,7 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>1338</v>
+        <v>815</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1100,16 +1100,16 @@
         </is>
       </c>
       <c r="C26">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>carpeta</t>
+          <t>esperma</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>carpeta</t>
+          <t>esperma</t>
         </is>
       </c>
       <c r="F26">
@@ -1121,7 +1121,7 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>883</v>
+        <v>924</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1129,20 +1129,20 @@
         </is>
       </c>
       <c r="C27">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>cate</t>
+          <t>emisión</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>cate, cate</t>
+          <t>emisión</t>
         </is>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>1272</v>
+        <v>994</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1158,28 +1158,28 @@
         </is>
       </c>
       <c r="C28">
-        <v>19</v>
+        <v>198</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>esperma</t>
+          <t>superioridad</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>esterma, esterma</t>
+          <t>superioridad</t>
         </is>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>1811</v>
+        <v>1835</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1187,28 +1187,28 @@
         </is>
       </c>
       <c r="C29">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>platillo</t>
+          <t>quejido</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>platillo</t>
+          <t>tejido</t>
         </is>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>1838</v>
+        <v>1856</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1216,16 +1216,16 @@
         </is>
       </c>
       <c r="C30">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>patente</t>
+          <t>destello</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>patente</t>
+          <t>destello</t>
         </is>
       </c>
       <c r="F30">
@@ -1237,7 +1237,7 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>1796</v>
+        <v>1862</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1245,16 +1245,16 @@
         </is>
       </c>
       <c r="C31">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>ceniza</t>
+          <t>tocador</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>ceniza</t>
+          <t>tocador</t>
         </is>
       </c>
       <c r="F31">
@@ -1266,7 +1266,7 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>1851</v>
+        <v>1865</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1274,28 +1274,28 @@
         </is>
       </c>
       <c r="C32">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>desazón</t>
+          <t>léxico</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>desazón</t>
+          <t>léstico</t>
         </is>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>1854</v>
+        <v>1801</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1303,20 +1303,20 @@
         </is>
       </c>
       <c r="C33">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>frescor</t>
+          <t>merluza</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>fres, frescor</t>
+          <t>merluza</t>
         </is>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>1802</v>
+        <v>1836</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1332,20 +1332,20 @@
         </is>
       </c>
       <c r="C34">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>temblor</t>
+          <t>ventanal</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>tel, temblor</t>
+          <t>ventanal</t>
         </is>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -1353,7 +1353,7 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>1805</v>
+        <v>1852</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1361,20 +1361,20 @@
         </is>
       </c>
       <c r="C35">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>neutrón</t>
+          <t>pilares</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>i, neutrón</t>
+          <t>pilares</t>
         </is>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>1826</v>
+        <v>1849</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1390,16 +1390,16 @@
         </is>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>bosnios</t>
+          <t>delirio</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>bosnios</t>
+          <t>delirio</t>
         </is>
       </c>
       <c r="F36">
@@ -1411,7 +1411,7 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>1794</v>
+        <v>1859</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1419,16 +1419,16 @@
         </is>
       </c>
       <c r="C37">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>islam</t>
+          <t>capellán</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>islam</t>
+          <t>capellán</t>
         </is>
       </c>
       <c r="F37">

</xml_diff>